<commit_message>
actualización  + test object upload
</commit_message>
<xml_diff>
--- a/ine_ipc_nacional.xlsx
+++ b/ine_ipc_nacional.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E253"/>
+  <dimension ref="A1:E254"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4748,6 +4748,23 @@
         <v>20.39958998393185</v>
       </c>
     </row>
+    <row r="254">
+      <c r="A254" s="2" t="n">
+        <v>46023</v>
+      </c>
+      <c r="B254" t="n">
+        <v>149.0611704407</v>
+      </c>
+      <c r="C254" t="n">
+        <v>1.308109633700494</v>
+      </c>
+      <c r="D254" t="n">
+        <v>1.308109633700494</v>
+      </c>
+      <c r="E254" t="n">
+        <v>19.63693943482947</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>